<commit_message>
novy design od Alese
</commit_message>
<xml_diff>
--- a/documents/Olympia 2018_startovka.xlsx
+++ b/documents/Olympia 2018_startovka.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\XAMPP\App\xampp\htdocs\splh\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\splh2\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87776623-A300-44F0-9B82-3641866F3172}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="300" yWindow="4215" windowWidth="21600" windowHeight="11385"/>
+    <workbookView xWindow="3195" yWindow="3105" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="muži" sheetId="1" r:id="rId1"/>
@@ -21,7 +22,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">muži!$A$2:$K$18</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -279,7 +280,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -440,7 +441,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="5">
-    <cellStyle name="40 % – Zvýraznění4" xfId="2" builtinId="43"/>
+    <cellStyle name="40 % – Zvýraznění 4" xfId="2" builtinId="43"/>
     <cellStyle name="Neutrální" xfId="4" builtinId="28"/>
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
     <cellStyle name="Správně" xfId="3" builtinId="26"/>
@@ -721,11 +722,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -785,14 +786,16 @@
         <v>6.2</v>
       </c>
       <c r="E2" s="7">
-        <v>1.25</v>
-      </c>
-      <c r="F2" s="7"/>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F2" s="7">
+        <v>1.2</v>
+      </c>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
       <c r="I2" s="8">
         <f t="shared" ref="I2" si="0">IF(E2+F2+G2+H2=0," ",MIN(E2:H2))</f>
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J2" s="8"/>
       <c r="K2" s="1">
@@ -814,19 +817,21 @@
         <v>6.9</v>
       </c>
       <c r="E3" s="7">
-        <v>1.25</v>
-      </c>
-      <c r="F3" s="7"/>
+        <v>5.6</v>
+      </c>
+      <c r="F3" s="7">
+        <v>0</v>
+      </c>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
       <c r="I3" s="8">
         <f t="shared" ref="I3:I18" si="2">IF(E3+F3+G3+H3=0," ",MIN(E3:H3))</f>
-        <v>1.25</v>
+        <v>0</v>
       </c>
       <c r="J3" s="8"/>
       <c r="K3" s="1">
         <f t="shared" ref="K3:K18" si="3">IF(I3=" "," ",_xlfn.RANK.EQ(I3,I$2:I$20,1))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -843,19 +848,19 @@
         <v>7</v>
       </c>
       <c r="E4" s="7">
-        <v>1.1399999999999999</v>
+        <v>12.5</v>
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
       <c r="I4" s="8">
         <f t="shared" si="2"/>
-        <v>1.1399999999999999</v>
+        <v>12.5</v>
       </c>
       <c r="J4" s="8"/>
       <c r="K4" s="1">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -871,18 +876,20 @@
       <c r="D5" s="2">
         <v>7.1</v>
       </c>
-      <c r="E5" s="7"/>
+      <c r="E5" s="7">
+        <v>12.5</v>
+      </c>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
-      <c r="I5" s="8" t="str">
+      <c r="I5" s="8">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
+        <v>12.5</v>
       </c>
       <c r="J5" s="8"/>
-      <c r="K5" s="1" t="str">
+      <c r="K5" s="1">
         <f t="shared" si="3"/>
-        <v xml:space="preserve"> </v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -898,18 +905,20 @@
       <c r="D6" s="2">
         <v>7.15</v>
       </c>
-      <c r="E6" s="7"/>
+      <c r="E6" s="7">
+        <v>12.5</v>
+      </c>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
-      <c r="I6" s="8" t="str">
+      <c r="I6" s="8">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
+        <v>12.5</v>
       </c>
       <c r="J6" s="8"/>
-      <c r="K6" s="1" t="str">
+      <c r="K6" s="1">
         <f t="shared" si="3"/>
-        <v xml:space="preserve"> </v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -925,18 +934,20 @@
       <c r="D7" s="2">
         <v>7.2</v>
       </c>
-      <c r="E7" s="7"/>
+      <c r="E7" s="7">
+        <v>12.5</v>
+      </c>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
-      <c r="I7" s="8" t="str">
+      <c r="I7" s="8">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
+        <v>12.5</v>
       </c>
       <c r="J7" s="8"/>
-      <c r="K7" s="1" t="str">
+      <c r="K7" s="1">
         <f t="shared" si="3"/>
-        <v xml:space="preserve"> </v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -952,18 +963,20 @@
       <c r="D8" s="2">
         <v>7.5</v>
       </c>
-      <c r="E8" s="7"/>
+      <c r="E8" s="7">
+        <v>12.5</v>
+      </c>
       <c r="F8" s="7"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
-      <c r="I8" s="8" t="str">
+      <c r="I8" s="8">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
+        <v>12.5</v>
       </c>
       <c r="J8" s="8"/>
-      <c r="K8" s="1" t="str">
+      <c r="K8" s="1">
         <f t="shared" si="3"/>
-        <v xml:space="preserve"> </v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -979,18 +992,20 @@
       <c r="D9" s="2">
         <v>8</v>
       </c>
-      <c r="E9" s="7"/>
+      <c r="E9" s="7">
+        <v>12.5</v>
+      </c>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
-      <c r="I9" s="8" t="str">
+      <c r="I9" s="8">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
+        <v>12.5</v>
       </c>
       <c r="J9" s="17"/>
-      <c r="K9" s="1" t="str">
+      <c r="K9" s="1">
         <f t="shared" si="3"/>
-        <v xml:space="preserve"> </v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -1006,18 +1021,20 @@
       <c r="D10" s="2">
         <v>8.11</v>
       </c>
-      <c r="E10" s="7"/>
+      <c r="E10" s="7">
+        <v>12.5</v>
+      </c>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
-      <c r="I10" s="8" t="str">
+      <c r="I10" s="8">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
+        <v>12.5</v>
       </c>
       <c r="J10" s="8"/>
-      <c r="K10" s="1" t="str">
+      <c r="K10" s="1">
         <f t="shared" si="3"/>
-        <v xml:space="preserve"> </v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -1033,18 +1050,20 @@
       <c r="D11" s="2">
         <v>9.1999999999999993</v>
       </c>
-      <c r="E11" s="7"/>
+      <c r="E11" s="7">
+        <v>12.5</v>
+      </c>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
-      <c r="I11" s="8" t="str">
+      <c r="I11" s="8">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
+        <v>12.5</v>
       </c>
       <c r="J11" s="8"/>
-      <c r="K11" s="1" t="str">
+      <c r="K11" s="1">
         <f t="shared" si="3"/>
-        <v xml:space="preserve"> </v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -1060,18 +1079,20 @@
       <c r="D12" s="2">
         <v>9.1999999999999993</v>
       </c>
-      <c r="E12" s="7"/>
+      <c r="E12" s="7">
+        <v>12.5</v>
+      </c>
       <c r="F12" s="7"/>
       <c r="G12" s="9"/>
       <c r="H12" s="9"/>
-      <c r="I12" s="8" t="str">
+      <c r="I12" s="8">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
+        <v>12.5</v>
       </c>
       <c r="J12" s="8"/>
-      <c r="K12" s="1" t="str">
+      <c r="K12" s="1">
         <f t="shared" si="3"/>
-        <v xml:space="preserve"> </v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -1087,18 +1108,20 @@
       <c r="D13" s="2">
         <v>10</v>
       </c>
-      <c r="E13" s="7"/>
+      <c r="E13" s="7">
+        <v>12.5</v>
+      </c>
       <c r="F13" s="7"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
-      <c r="I13" s="8" t="str">
+      <c r="I13" s="8">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
+        <v>12.5</v>
       </c>
       <c r="J13" s="8"/>
-      <c r="K13" s="1" t="str">
+      <c r="K13" s="1">
         <f t="shared" si="3"/>
-        <v xml:space="preserve"> </v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -1114,18 +1137,20 @@
       <c r="D14" s="2">
         <v>11</v>
       </c>
-      <c r="E14" s="7"/>
+      <c r="E14" s="7">
+        <v>12.5</v>
+      </c>
       <c r="F14" s="7"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
-      <c r="I14" s="8" t="str">
+      <c r="I14" s="8">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
+        <v>12.5</v>
       </c>
       <c r="J14" s="8"/>
-      <c r="K14" s="1" t="str">
+      <c r="K14" s="1">
         <f t="shared" si="3"/>
-        <v xml:space="preserve"> </v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -1141,20 +1166,22 @@
       <c r="D15" s="2">
         <v>12.5</v>
       </c>
-      <c r="E15" s="7"/>
+      <c r="E15" s="7">
+        <v>12.5</v>
+      </c>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
-      <c r="I15" s="8" t="str">
+      <c r="I15" s="8">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
+        <v>12.5</v>
       </c>
       <c r="J15" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="K15" s="1" t="str">
+      <c r="K15" s="1">
         <f t="shared" si="3"/>
-        <v xml:space="preserve"> </v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -1170,18 +1197,20 @@
       <c r="D16" s="2">
         <v>12.5</v>
       </c>
-      <c r="E16" s="7"/>
+      <c r="E16" s="7">
+        <v>12.5</v>
+      </c>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
-      <c r="I16" s="8" t="str">
+      <c r="I16" s="8">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
+        <v>12.5</v>
       </c>
       <c r="J16" s="8"/>
-      <c r="K16" s="1" t="str">
+      <c r="K16" s="1">
         <f t="shared" si="3"/>
-        <v xml:space="preserve"> </v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -1197,18 +1226,20 @@
       <c r="D17" s="2">
         <v>15</v>
       </c>
-      <c r="E17" s="7"/>
+      <c r="E17" s="7">
+        <v>12.5</v>
+      </c>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
-      <c r="I17" s="8" t="str">
+      <c r="I17" s="8">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
+        <v>12.5</v>
       </c>
       <c r="J17" s="8"/>
-      <c r="K17" s="1" t="str">
+      <c r="K17" s="1">
         <f t="shared" si="3"/>
-        <v xml:space="preserve"> </v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -1224,18 +1255,20 @@
       <c r="D18" s="2">
         <v>16.11</v>
       </c>
-      <c r="E18" s="7"/>
+      <c r="E18" s="7">
+        <v>12.5</v>
+      </c>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
       <c r="H18" s="7"/>
-      <c r="I18" s="8" t="str">
+      <c r="I18" s="8">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
+        <v>12.5</v>
       </c>
       <c r="J18" s="8"/>
-      <c r="K18" s="1" t="str">
+      <c r="K18" s="1">
         <f t="shared" si="3"/>
-        <v xml:space="preserve"> </v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -1279,7 +1312,7 @@
       <c r="K22" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:K18">
+  <autoFilter ref="A2:K18" xr:uid="{3A5B869D-E47E-4649-B5B0-387EF1D71CFA}">
     <sortState ref="A3:K18">
       <sortCondition ref="D2:D18"/>
     </sortState>
@@ -1297,11 +1330,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1367,11 +1400,11 @@
         <v>888</v>
       </c>
       <c r="H2" s="7">
-        <v>888</v>
+        <v>0</v>
       </c>
       <c r="I2" s="8">
         <f>IF(E2+F2+G2+H2=0," ",MIN(E2:H2))</f>
-        <v>888</v>
+        <v>0</v>
       </c>
       <c r="J2" s="1">
         <v>2</v>
@@ -1399,9 +1432,7 @@
       <c r="G3" s="1">
         <v>888</v>
       </c>
-      <c r="H3" s="1">
-        <v>888</v>
-      </c>
+      <c r="H3" s="1"/>
       <c r="I3" s="8">
         <f>IF(E3+F3+G3+H3=0," ",MIN(E3:H3))</f>
         <v>36</v>
@@ -1580,7 +1611,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
@@ -2123,7 +2154,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
@@ -2642,7 +2673,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView showRowColHeaders="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">

</xml_diff>

<commit_message>
nadpis tabulky, bootstrap 4.0.0
</commit_message>
<xml_diff>
--- a/documents/Olympia 2018_startovka.xlsx
+++ b/documents/Olympia 2018_startovka.xlsx
@@ -1,28 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\splh2\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jirka\Home\splh\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87776623-A300-44F0-9B82-3641866F3172}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3195" yWindow="3105" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3195" yWindow="3105" windowWidth="21600" windowHeight="11385"/>
   </bookViews>
   <sheets>
-    <sheet name="muži" sheetId="1" r:id="rId1"/>
-    <sheet name="Masters" sheetId="6" r:id="rId2"/>
-    <sheet name="dorostenci" sheetId="2" r:id="rId3"/>
+    <sheet name="dorostenci" sheetId="2" r:id="rId1"/>
+    <sheet name="muži" sheetId="1" r:id="rId2"/>
+    <sheet name="Masters" sheetId="6" r:id="rId3"/>
     <sheet name="žáci" sheetId="3" r:id="rId4"/>
     <sheet name="ženy" sheetId="4" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">muži!$A$2:$K$18</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">muži!$A$2:$K$18</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="74">
   <si>
     <t>jméno</t>
   </si>
@@ -276,11 +275,14 @@
   <si>
     <t>Nantl Jan</t>
   </si>
+  <si>
+    <t>KONEC 1. kola</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -441,7 +443,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="5">
-    <cellStyle name="40 % – Zvýraznění 4" xfId="2" builtinId="43"/>
+    <cellStyle name="40 % – Zvýraznění4" xfId="2" builtinId="43"/>
     <cellStyle name="Neutrální" xfId="4" builtinId="28"/>
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
     <cellStyle name="Správně" xfId="3" builtinId="26"/>
@@ -722,11 +724,526 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.5703125" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="4">
+        <v>2001</v>
+      </c>
+      <c r="D2" s="2">
+        <v>4</v>
+      </c>
+      <c r="E2" s="7">
+        <v>4.18</v>
+      </c>
+      <c r="F2" s="7">
+        <v>4.0199999999999996</v>
+      </c>
+      <c r="G2" s="7">
+        <v>4.07</v>
+      </c>
+      <c r="H2" s="11">
+        <v>4.6399999999999997</v>
+      </c>
+      <c r="I2" s="8">
+        <f t="shared" ref="I2:I12" si="0">IF(E2+F2+G2+H2=0," ",MIN(E2:H2))</f>
+        <v>4.0199999999999996</v>
+      </c>
+      <c r="J2" s="1">
+        <f t="shared" ref="J2:J12" si="1">IF(I2=" "," ",_xlfn.RANK.EQ(I2,I$2:I$18,1))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="4">
+        <v>2001</v>
+      </c>
+      <c r="D3" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="E3" s="7">
+        <v>4.29</v>
+      </c>
+      <c r="F3" s="7">
+        <v>4.17</v>
+      </c>
+      <c r="G3" s="7">
+        <v>4.04</v>
+      </c>
+      <c r="H3" s="11">
+        <v>4.16</v>
+      </c>
+      <c r="I3" s="8">
+        <f t="shared" si="0"/>
+        <v>4.04</v>
+      </c>
+      <c r="J3" s="1">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="4">
+        <v>2001</v>
+      </c>
+      <c r="D4" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="E4" s="7">
+        <v>4.76</v>
+      </c>
+      <c r="F4" s="7">
+        <v>4.3499999999999996</v>
+      </c>
+      <c r="G4" s="7">
+        <v>999</v>
+      </c>
+      <c r="H4" s="11">
+        <v>4.58</v>
+      </c>
+      <c r="I4" s="8">
+        <f t="shared" si="0"/>
+        <v>4.3499999999999996</v>
+      </c>
+      <c r="J4" s="1">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="4">
+        <v>2001</v>
+      </c>
+      <c r="D5" s="2">
+        <v>5</v>
+      </c>
+      <c r="E5" s="7">
+        <v>4.71</v>
+      </c>
+      <c r="F5" s="7">
+        <v>4.46</v>
+      </c>
+      <c r="G5" s="7">
+        <v>4.58</v>
+      </c>
+      <c r="H5" s="11">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="I5" s="8">
+        <f t="shared" si="0"/>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="J5" s="1">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="4">
+        <v>2001</v>
+      </c>
+      <c r="D6" s="2">
+        <v>5</v>
+      </c>
+      <c r="E6" s="7">
+        <v>5.54</v>
+      </c>
+      <c r="F6" s="7">
+        <v>4.66</v>
+      </c>
+      <c r="G6" s="7"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="8">
+        <f t="shared" si="0"/>
+        <v>4.66</v>
+      </c>
+      <c r="J6" s="1">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="4">
+        <v>2000</v>
+      </c>
+      <c r="D7" s="2">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="E7" s="7">
+        <v>4.5</v>
+      </c>
+      <c r="F7" s="7">
+        <v>4.6900000000000004</v>
+      </c>
+      <c r="G7" s="7"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="8">
+        <f t="shared" si="0"/>
+        <v>4.5</v>
+      </c>
+      <c r="J7" s="1">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="4">
+        <v>2002</v>
+      </c>
+      <c r="D8" s="2">
+        <v>4.7</v>
+      </c>
+      <c r="E8" s="7">
+        <v>4.72</v>
+      </c>
+      <c r="F8" s="7">
+        <v>4.6500000000000004</v>
+      </c>
+      <c r="G8" s="7"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="8">
+        <f t="shared" si="0"/>
+        <v>4.6500000000000004</v>
+      </c>
+      <c r="J8" s="1">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="4">
+        <v>2001</v>
+      </c>
+      <c r="D9" s="2">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="E9" s="7">
+        <v>5.17</v>
+      </c>
+      <c r="F9" s="7">
+        <v>4.66</v>
+      </c>
+      <c r="G9" s="7"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="8">
+        <f t="shared" si="0"/>
+        <v>4.66</v>
+      </c>
+      <c r="J9" s="1">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="4">
+        <v>2002</v>
+      </c>
+      <c r="D10" s="2">
+        <v>5.5</v>
+      </c>
+      <c r="E10" s="7">
+        <v>5.32</v>
+      </c>
+      <c r="F10" s="7">
+        <v>6.04</v>
+      </c>
+      <c r="G10" s="7"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="8">
+        <f t="shared" si="0"/>
+        <v>5.32</v>
+      </c>
+      <c r="J10" s="1">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="4">
+        <v>2001</v>
+      </c>
+      <c r="D11" s="2">
+        <v>6.3</v>
+      </c>
+      <c r="E11" s="13">
+        <v>5.84</v>
+      </c>
+      <c r="F11" s="7">
+        <v>5.87</v>
+      </c>
+      <c r="G11" s="7"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="8">
+        <f t="shared" si="0"/>
+        <v>5.84</v>
+      </c>
+      <c r="J11" s="1">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="4">
+        <v>2002</v>
+      </c>
+      <c r="D12" s="2">
+        <v>6.4</v>
+      </c>
+      <c r="E12" s="7">
+        <v>999</v>
+      </c>
+      <c r="F12" s="7">
+        <v>6.15</v>
+      </c>
+      <c r="G12" s="7"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="8">
+        <f t="shared" si="0"/>
+        <v>6.15</v>
+      </c>
+      <c r="J12" s="1">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="1"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="1"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="1"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="1"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="1"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="1"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="1"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="1"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="1"/>
+    </row>
+  </sheetData>
+  <sortState ref="A2:J12">
+    <sortCondition ref="I2:I12"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"-,Tučné"&amp;UŠplh v Olympii&amp;U (dorostenci)
+&amp;"-,Obyčejné"21. 4. 2018</oddHeader>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -789,18 +1306,18 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="F2" s="7">
-        <v>1.2</v>
+        <v>12.23</v>
       </c>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
       <c r="I2" s="8">
         <f t="shared" ref="I2" si="0">IF(E2+F2+G2+H2=0," ",MIN(E2:H2))</f>
-        <v>1.2</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="J2" s="8"/>
       <c r="K2" s="1">
         <f t="shared" ref="K2" si="1">IF(I2=" "," ",_xlfn.RANK.EQ(I2,I$2:I$20,1))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -820,18 +1337,18 @@
         <v>5.6</v>
       </c>
       <c r="F3" s="7">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
       <c r="I3" s="8">
-        <f t="shared" ref="I3:I18" si="2">IF(E3+F3+G3+H3=0," ",MIN(E3:H3))</f>
-        <v>0</v>
+        <f t="shared" ref="I3:I19" si="2">IF(E3+F3+G3+H3=0," ",MIN(E3:H3))</f>
+        <v>5.6</v>
       </c>
       <c r="J3" s="8"/>
       <c r="K3" s="1">
         <f t="shared" ref="K3:K18" si="3">IF(I3=" "," ",_xlfn.RANK.EQ(I3,I$2:I$20,1))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -850,7 +1367,9 @@
       <c r="E4" s="7">
         <v>12.5</v>
       </c>
-      <c r="F4" s="7"/>
+      <c r="F4" s="7">
+        <v>13</v>
+      </c>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
       <c r="I4" s="8">
@@ -860,7 +1379,7 @@
       <c r="J4" s="8"/>
       <c r="K4" s="1">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -879,7 +1398,9 @@
       <c r="E5" s="7">
         <v>12.5</v>
       </c>
-      <c r="F5" s="7"/>
+      <c r="F5" s="7">
+        <v>14</v>
+      </c>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
       <c r="I5" s="8">
@@ -889,7 +1410,7 @@
       <c r="J5" s="8"/>
       <c r="K5" s="1">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -908,7 +1429,9 @@
       <c r="E6" s="7">
         <v>12.5</v>
       </c>
-      <c r="F6" s="7"/>
+      <c r="F6" s="7">
+        <v>15</v>
+      </c>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
       <c r="I6" s="8">
@@ -918,7 +1441,7 @@
       <c r="J6" s="8"/>
       <c r="K6" s="1">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -937,7 +1460,9 @@
       <c r="E7" s="7">
         <v>12.5</v>
       </c>
-      <c r="F7" s="7"/>
+      <c r="F7" s="7">
+        <v>13</v>
+      </c>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
       <c r="I7" s="8">
@@ -947,7 +1472,7 @@
       <c r="J7" s="8"/>
       <c r="K7" s="1">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -966,17 +1491,19 @@
       <c r="E8" s="7">
         <v>12.5</v>
       </c>
-      <c r="F8" s="7"/>
+      <c r="F8" s="7">
+        <v>11.12</v>
+      </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="8">
         <f t="shared" si="2"/>
-        <v>12.5</v>
+        <v>11.12</v>
       </c>
       <c r="J8" s="8"/>
       <c r="K8" s="1">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -995,12 +1522,14 @@
       <c r="E9" s="7">
         <v>12.5</v>
       </c>
-      <c r="F9" s="7"/>
+      <c r="F9" s="7">
+        <v>10</v>
+      </c>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
       <c r="I9" s="8">
         <f t="shared" si="2"/>
-        <v>12.5</v>
+        <v>10</v>
       </c>
       <c r="J9" s="17"/>
       <c r="K9" s="1">
@@ -1024,12 +1553,14 @@
       <c r="E10" s="7">
         <v>12.5</v>
       </c>
-      <c r="F10" s="7"/>
+      <c r="F10" s="7">
+        <v>10</v>
+      </c>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
       <c r="I10" s="8">
         <f t="shared" si="2"/>
-        <v>12.5</v>
+        <v>10</v>
       </c>
       <c r="J10" s="8"/>
       <c r="K10" s="1">
@@ -1053,12 +1584,14 @@
       <c r="E11" s="7">
         <v>12.5</v>
       </c>
-      <c r="F11" s="7"/>
+      <c r="F11" s="7">
+        <v>10</v>
+      </c>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
       <c r="I11" s="8">
         <f t="shared" si="2"/>
-        <v>12.5</v>
+        <v>10</v>
       </c>
       <c r="J11" s="8"/>
       <c r="K11" s="1">
@@ -1082,12 +1615,14 @@
       <c r="E12" s="7">
         <v>12.5</v>
       </c>
-      <c r="F12" s="7"/>
+      <c r="F12" s="7">
+        <v>10</v>
+      </c>
       <c r="G12" s="9"/>
       <c r="H12" s="9"/>
       <c r="I12" s="8">
         <f t="shared" si="2"/>
-        <v>12.5</v>
+        <v>10</v>
       </c>
       <c r="J12" s="8"/>
       <c r="K12" s="1">
@@ -1111,17 +1646,19 @@
       <c r="E13" s="7">
         <v>12.5</v>
       </c>
-      <c r="F13" s="7"/>
+      <c r="F13" s="7">
+        <v>11</v>
+      </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="8">
         <f t="shared" si="2"/>
-        <v>12.5</v>
+        <v>11</v>
       </c>
       <c r="J13" s="8"/>
       <c r="K13" s="1">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -1140,17 +1677,19 @@
       <c r="E14" s="7">
         <v>12.5</v>
       </c>
-      <c r="F14" s="7"/>
+      <c r="F14" s="7">
+        <v>12</v>
+      </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="8">
         <f t="shared" si="2"/>
-        <v>12.5</v>
+        <v>12</v>
       </c>
       <c r="J14" s="8"/>
       <c r="K14" s="1">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -1169,19 +1708,21 @@
       <c r="E15" s="7">
         <v>12.5</v>
       </c>
-      <c r="F15" s="7"/>
+      <c r="F15" s="7">
+        <v>12</v>
+      </c>
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
       <c r="I15" s="8">
         <f t="shared" si="2"/>
-        <v>12.5</v>
+        <v>12</v>
       </c>
       <c r="J15" s="17" t="s">
         <v>33</v>
       </c>
       <c r="K15" s="1">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -1200,7 +1741,9 @@
       <c r="E16" s="7">
         <v>12.5</v>
       </c>
-      <c r="F16" s="7"/>
+      <c r="F16" s="7">
+        <v>14</v>
+      </c>
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
       <c r="I16" s="8">
@@ -1210,7 +1753,7 @@
       <c r="J16" s="8"/>
       <c r="K16" s="1">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -1229,7 +1772,9 @@
       <c r="E17" s="7">
         <v>12.5</v>
       </c>
-      <c r="F17" s="7"/>
+      <c r="F17" s="7">
+        <v>19</v>
+      </c>
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
       <c r="I17" s="8">
@@ -1239,7 +1784,7 @@
       <c r="J17" s="8"/>
       <c r="K17" s="1">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -1268,15 +1813,21 @@
       <c r="J18" s="8"/>
       <c r="K18" s="1">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
+      <c r="A19" s="3" t="s">
+        <v>73</v>
+      </c>
       <c r="B19" s="1"/>
       <c r="C19" s="4"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="7"/>
+      <c r="D19" s="2">
+        <v>0</v>
+      </c>
+      <c r="E19" s="7">
+        <v>0</v>
+      </c>
       <c r="F19" s="16"/>
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
@@ -1312,7 +1863,7 @@
       <c r="K22" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:K18" xr:uid="{3A5B869D-E47E-4649-B5B0-387EF1D71CFA}">
+  <autoFilter ref="A2:K18">
     <sortState ref="A3:K18">
       <sortCondition ref="D2:D18"/>
     </sortState>
@@ -1329,8 +1880,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
@@ -1610,551 +2161,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:J21"/>
-  <sheetViews>
-    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:J22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="22.5703125" customWidth="1"/>
-    <col min="2" max="2" width="20.140625" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" customWidth="1"/>
-    <col min="9" max="9" width="12.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="4">
-        <v>2001</v>
-      </c>
-      <c r="D2" s="2">
-        <v>4</v>
-      </c>
-      <c r="E2" s="7">
-        <v>4.18</v>
-      </c>
-      <c r="F2" s="7">
-        <v>4.0199999999999996</v>
-      </c>
-      <c r="G2" s="7">
-        <v>4.07</v>
-      </c>
-      <c r="H2" s="11">
-        <v>4.6399999999999997</v>
-      </c>
-      <c r="I2" s="8">
-        <f t="shared" ref="I2:I12" si="0">IF(E2+F2+G2+H2=0," ",MIN(E2:H2))</f>
-        <v>4.0199999999999996</v>
-      </c>
-      <c r="J2" s="1">
-        <f t="shared" ref="J2:J12" si="1">IF(I2=" "," ",_xlfn.RANK.EQ(I2,I$2:I$18,1))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="4">
-        <v>2001</v>
-      </c>
-      <c r="D3" s="2">
-        <v>4.5</v>
-      </c>
-      <c r="E3" s="7">
-        <v>4.29</v>
-      </c>
-      <c r="F3" s="7">
-        <v>4.17</v>
-      </c>
-      <c r="G3" s="7">
-        <v>4.04</v>
-      </c>
-      <c r="H3" s="11">
-        <v>4.16</v>
-      </c>
-      <c r="I3" s="8">
-        <f t="shared" si="0"/>
-        <v>4.04</v>
-      </c>
-      <c r="J3" s="1">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="4">
-        <v>2001</v>
-      </c>
-      <c r="D4" s="2">
-        <v>4.5</v>
-      </c>
-      <c r="E4" s="7">
-        <v>4.76</v>
-      </c>
-      <c r="F4" s="7">
-        <v>4.3499999999999996</v>
-      </c>
-      <c r="G4" s="7">
-        <v>999</v>
-      </c>
-      <c r="H4" s="11">
-        <v>4.58</v>
-      </c>
-      <c r="I4" s="8">
-        <f t="shared" si="0"/>
-        <v>4.3499999999999996</v>
-      </c>
-      <c r="J4" s="1">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="4">
-        <v>2001</v>
-      </c>
-      <c r="D5" s="2">
-        <v>5</v>
-      </c>
-      <c r="E5" s="7">
-        <v>4.71</v>
-      </c>
-      <c r="F5" s="7">
-        <v>4.46</v>
-      </c>
-      <c r="G5" s="7">
-        <v>4.58</v>
-      </c>
-      <c r="H5" s="11">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="I5" s="8">
-        <f t="shared" si="0"/>
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="J5" s="1">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="4">
-        <v>2001</v>
-      </c>
-      <c r="D6" s="2">
-        <v>5</v>
-      </c>
-      <c r="E6" s="7">
-        <v>5.54</v>
-      </c>
-      <c r="F6" s="7">
-        <v>4.66</v>
-      </c>
-      <c r="G6" s="7">
-        <v>4.43</v>
-      </c>
-      <c r="H6" s="11">
-        <v>5.18</v>
-      </c>
-      <c r="I6" s="8">
-        <f t="shared" si="0"/>
-        <v>4.43</v>
-      </c>
-      <c r="J6" s="1">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C7" s="4">
-        <v>2000</v>
-      </c>
-      <c r="D7" s="2">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="E7" s="7">
-        <v>4.5</v>
-      </c>
-      <c r="F7" s="7">
-        <v>4.6900000000000004</v>
-      </c>
-      <c r="G7" s="7">
-        <v>4.8899999999999997</v>
-      </c>
-      <c r="H7" s="11">
-        <v>4.76</v>
-      </c>
-      <c r="I7" s="8">
-        <f t="shared" si="0"/>
-        <v>4.5</v>
-      </c>
-      <c r="J7" s="1">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="4">
-        <v>2002</v>
-      </c>
-      <c r="D8" s="2">
-        <v>4.7</v>
-      </c>
-      <c r="E8" s="7">
-        <v>4.72</v>
-      </c>
-      <c r="F8" s="7">
-        <v>4.6500000000000004</v>
-      </c>
-      <c r="G8" s="7">
-        <v>4.68</v>
-      </c>
-      <c r="H8" s="11">
-        <v>6.6</v>
-      </c>
-      <c r="I8" s="8">
-        <f t="shared" si="0"/>
-        <v>4.6500000000000004</v>
-      </c>
-      <c r="J8" s="1">
-        <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="4">
-        <v>2001</v>
-      </c>
-      <c r="D9" s="2">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="E9" s="7">
-        <v>5.17</v>
-      </c>
-      <c r="F9" s="7">
-        <v>4.66</v>
-      </c>
-      <c r="G9" s="7">
-        <v>5</v>
-      </c>
-      <c r="H9" s="11">
-        <v>5.05</v>
-      </c>
-      <c r="I9" s="8">
-        <f t="shared" si="0"/>
-        <v>4.66</v>
-      </c>
-      <c r="J9" s="1">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="4">
-        <v>2002</v>
-      </c>
-      <c r="D10" s="2">
-        <v>5.5</v>
-      </c>
-      <c r="E10" s="7">
-        <v>5.32</v>
-      </c>
-      <c r="F10" s="7">
-        <v>6.04</v>
-      </c>
-      <c r="G10" s="7">
-        <v>5.35</v>
-      </c>
-      <c r="H10" s="11">
-        <v>5.35</v>
-      </c>
-      <c r="I10" s="8">
-        <f t="shared" si="0"/>
-        <v>5.32</v>
-      </c>
-      <c r="J10" s="1">
-        <f t="shared" si="1"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="4">
-        <v>2001</v>
-      </c>
-      <c r="D11" s="2">
-        <v>6.3</v>
-      </c>
-      <c r="E11" s="13">
-        <v>5.84</v>
-      </c>
-      <c r="F11" s="7">
-        <v>5.87</v>
-      </c>
-      <c r="G11" s="7">
-        <v>6.1</v>
-      </c>
-      <c r="H11" s="11">
-        <v>5.59</v>
-      </c>
-      <c r="I11" s="8">
-        <f t="shared" si="0"/>
-        <v>5.59</v>
-      </c>
-      <c r="J11" s="1">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="4">
-        <v>2002</v>
-      </c>
-      <c r="D12" s="2">
-        <v>6.4</v>
-      </c>
-      <c r="E12" s="7">
-        <v>999</v>
-      </c>
-      <c r="F12" s="7">
-        <v>6.15</v>
-      </c>
-      <c r="G12" s="7">
-        <v>6.06</v>
-      </c>
-      <c r="H12" s="11">
-        <v>5.75</v>
-      </c>
-      <c r="I12" s="8">
-        <f t="shared" si="0"/>
-        <v>5.75</v>
-      </c>
-      <c r="J12" s="1">
-        <f t="shared" si="1"/>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="1"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="1"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="1"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="1"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="1"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="1"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="1"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="1"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="8"/>
-      <c r="J21" s="1"/>
-    </row>
-  </sheetData>
-  <sortState ref="A2:J12">
-    <sortCondition ref="I2:I12"/>
-  </sortState>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
-  <headerFooter>
-    <oddHeader>&amp;C&amp;"-,Tučné"&amp;UŠplh v Olympii&amp;U (dorostenci)
-&amp;"-,Obyčejné"21. 4. 2018</oddHeader>
-  </headerFooter>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
@@ -2673,7 +2681,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView showRowColHeaders="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">

</xml_diff>

<commit_message>
local css and js
</commit_message>
<xml_diff>
--- a/documents/Olympia 2018_startovka.xlsx
+++ b/documents/Olympia 2018_startovka.xlsx
@@ -728,7 +728,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -926,7 +926,9 @@
       <c r="F6" s="7">
         <v>4.66</v>
       </c>
-      <c r="G6" s="7"/>
+      <c r="G6" s="7">
+        <v>12</v>
+      </c>
       <c r="H6" s="11"/>
       <c r="I6" s="8">
         <f t="shared" si="0"/>
@@ -956,7 +958,9 @@
       <c r="F7" s="7">
         <v>4.6900000000000004</v>
       </c>
-      <c r="G7" s="7"/>
+      <c r="G7" s="7">
+        <v>4.6900000000000004</v>
+      </c>
       <c r="H7" s="11"/>
       <c r="I7" s="8">
         <f t="shared" si="0"/>
@@ -986,7 +990,9 @@
       <c r="F8" s="7">
         <v>4.6500000000000004</v>
       </c>
-      <c r="G8" s="7"/>
+      <c r="G8" s="7">
+        <v>4.6900000000000004</v>
+      </c>
       <c r="H8" s="11"/>
       <c r="I8" s="8">
         <f t="shared" si="0"/>
@@ -1016,7 +1022,9 @@
       <c r="F9" s="7">
         <v>4.66</v>
       </c>
-      <c r="G9" s="7"/>
+      <c r="G9" s="7">
+        <v>4.6900000000000004</v>
+      </c>
       <c r="H9" s="11"/>
       <c r="I9" s="8">
         <f t="shared" si="0"/>
@@ -1046,11 +1054,13 @@
       <c r="F10" s="7">
         <v>6.04</v>
       </c>
-      <c r="G10" s="7"/>
+      <c r="G10" s="7">
+        <v>4.6900000000000004</v>
+      </c>
       <c r="H10" s="11"/>
       <c r="I10" s="8">
         <f t="shared" si="0"/>
-        <v>5.32</v>
+        <v>4.6900000000000004</v>
       </c>
       <c r="J10" s="1">
         <f t="shared" si="1"/>
@@ -1076,15 +1086,17 @@
       <c r="F11" s="7">
         <v>5.87</v>
       </c>
-      <c r="G11" s="7"/>
+      <c r="G11" s="7">
+        <v>4.6900000000000004</v>
+      </c>
       <c r="H11" s="11"/>
       <c r="I11" s="8">
         <f t="shared" si="0"/>
-        <v>5.84</v>
+        <v>4.6900000000000004</v>
       </c>
       <c r="J11" s="1">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -1106,15 +1118,17 @@
       <c r="F12" s="7">
         <v>6.15</v>
       </c>
-      <c r="G12" s="7"/>
+      <c r="G12" s="7">
+        <v>4.6900000000000004</v>
+      </c>
       <c r="H12" s="11"/>
       <c r="I12" s="8">
         <f t="shared" si="0"/>
-        <v>6.15</v>
+        <v>4.6900000000000004</v>
       </c>
       <c r="J12" s="1">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -1342,7 +1356,7 @@
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
       <c r="I3" s="8">
-        <f t="shared" ref="I3:I19" si="2">IF(E3+F3+G3+H3=0," ",MIN(E3:H3))</f>
+        <f t="shared" ref="I3:I18" si="2">IF(E3+F3+G3+H3=0," ",MIN(E3:H3))</f>
         <v>5.6</v>
       </c>
       <c r="J3" s="8"/>

</xml_diff>